<commit_message>
Update RNAi_survival - gene and virus.xlsx
</commit_message>
<xml_diff>
--- a/data/RNAi_survival - gene and virus.xlsx
+++ b/data/RNAi_survival - gene and virus.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/Documents/GitHub/varroa-virus-knockdown/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4347484-C55E-424E-8788-637043EA65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8774925-92BB-B34B-A075-FA68E8DDF3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{842BBCB6-D410-CB4F-9404-EF737D3C039C}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="29920" windowHeight="21100" activeTab="1" xr2:uid="{842BBCB6-D410-CB4F-9404-EF737D3C039C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$B$43</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -116,6 +120,9 @@
   </si>
   <si>
     <t>gene-silence</t>
+  </si>
+  <si>
+    <t>survival_frq</t>
   </si>
 </sst>
 </file>
@@ -159,10 +166,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,15 +690,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65D4C80-DBDF-FD48-94B2-F2B58E58EE24}">
-  <dimension ref="A1:F43"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="163" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,29 +718,36 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44477</v>
+        <v>44551</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <f>F2-D2</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3">
+        <f>D2/F2</f>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44477</v>
       </c>
@@ -745,56 +761,68 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E27" si="0">F3-D3</f>
+        <f>F3-D3</f>
         <v>0</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="0">D3/F3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44477</v>
+        <v>44489</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
+        <f>F4-D4</f>
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44477</v>
+        <v>44490</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5">
+        <f>F5-D5</f>
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44477</v>
       </c>
@@ -808,14 +836,14 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>F6-D6</f>
         <v>0</v>
       </c>
       <c r="F6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44477</v>
       </c>
@@ -829,14 +857,14 @@
         <v>8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>F7-D7</f>
         <v>1</v>
       </c>
       <c r="F7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44477</v>
       </c>
@@ -850,14 +878,14 @@
         <v>9</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>F8-D8</f>
         <v>0</v>
       </c>
       <c r="F8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44477</v>
       </c>
@@ -871,14 +899,14 @@
         <v>6</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>F9-D9</f>
         <v>3</v>
       </c>
       <c r="F9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44477</v>
       </c>
@@ -892,37 +920,41 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>F10-D10</f>
         <v>1</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44489</v>
+        <v>44495</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
+      <c r="E11">
+        <f>F11-D11</f>
         <v>4</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="F11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="3">
+        <f t="shared" ref="G11:G13" si="1">D11/F11</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44489</v>
+        <v>44551</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -931,19 +963,23 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>F12-D12</f>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.88235294117647056</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44489</v>
+        <v>44477</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -952,17 +988,21 @@
         <v>25</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>F13-D13</f>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44489</v>
       </c>
@@ -976,14 +1016,14 @@
         <v>4</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>F14-D14</f>
         <v>5</v>
       </c>
       <c r="F14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44489</v>
       </c>
@@ -997,14 +1037,14 @@
         <v>6</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>F15-D15</f>
         <v>3</v>
       </c>
       <c r="F15">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44489</v>
       </c>
@@ -1018,58 +1058,66 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>F16-D16</f>
         <v>7</v>
       </c>
       <c r="F16">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44490</v>
+        <v>44489</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f>F17-D17</f>
         <v>6</v>
       </c>
       <c r="F17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="3">
+        <f t="shared" ref="G17:G19" si="2">D17/F17</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44490</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>F18-D18</f>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44490</v>
+        <v>44492</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -1078,17 +1126,21 @@
         <v>25</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>F19-D19</f>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44490</v>
       </c>
@@ -1102,14 +1154,14 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>F20-D20</f>
         <v>2</v>
       </c>
       <c r="F20">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44490</v>
       </c>
@@ -1123,16 +1175,16 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>F21-D21</f>
         <v>7</v>
       </c>
       <c r="F21">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44492</v>
+        <v>44477</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1141,38 +1193,46 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>F22-D22</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" ref="G22:G23" si="3">D22/F22</f>
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44492</v>
+        <v>44489</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>F23-D23</f>
+        <v>5</v>
       </c>
       <c r="F23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="3">
+        <f t="shared" si="3"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44492</v>
       </c>
@@ -1186,14 +1246,14 @@
         <v>5</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>F24-D24</f>
         <v>4</v>
       </c>
       <c r="F24">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44492</v>
       </c>
@@ -1207,14 +1267,14 @@
         <v>8</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f>F25-D25</f>
         <v>1</v>
       </c>
       <c r="F25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44492</v>
       </c>
@@ -1228,14 +1288,14 @@
         <v>5</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f>F26-D26</f>
         <v>4</v>
       </c>
       <c r="F26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44492</v>
       </c>
@@ -1256,15 +1316,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44492</v>
+        <v>44490</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1276,10 +1336,14 @@
       <c r="F28">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="3">
+        <f t="shared" ref="G28:G30" si="4">D28/F28</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44495</v>
+        <v>44492</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1288,38 +1352,46 @@
         <v>24</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E29">
         <f>F29-D29</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="3">
+        <f t="shared" si="4"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44495</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E30">
         <f>F30-D30</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="3">
+        <f t="shared" si="4"/>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44495</v>
       </c>
@@ -1340,7 +1412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44495</v>
       </c>
@@ -1361,7 +1433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44495</v>
       </c>
@@ -1382,7 +1454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44517</v>
       </c>
@@ -1402,8 +1474,12 @@
       <c r="F34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="3">
+        <f>D34/F34</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44517</v>
       </c>
@@ -1424,7 +1500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44517</v>
       </c>
@@ -1445,7 +1521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44517</v>
       </c>
@@ -1466,7 +1542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44517</v>
       </c>
@@ -1487,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44517</v>
       </c>
@@ -1508,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44551</v>
       </c>
@@ -1528,31 +1604,39 @@
       <c r="F40">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="3">
+        <f t="shared" ref="G40:G43" si="5">D40/F40</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44551</v>
+        <v>44477</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="D41">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <f>F41-D41</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44551</v>
+        <v>44492</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -1561,22 +1645,26 @@
         <v>25</v>
       </c>
       <c r="D42">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <f>F42-D42</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F42">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44551</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1591,8 +1679,26 @@
       <c r="F43">
         <v>18</v>
       </c>
+      <c r="G43" s="3">
+        <f t="shared" si="5"/>
+        <v>0.72222222222222221</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B43" xr:uid="{D65D4C80-DBDF-FD48-94B2-F2B58E58EE24}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ARV-2"/>
+        <filter val="DWVa"/>
+        <filter val="DWVb"/>
+        <filter val="GFP"/>
+        <filter val="VDV2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F43">
+    <sortCondition ref="B1:B43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>